<commit_message>
revisi BoM scada air
</commit_message>
<xml_diff>
--- a/BoM Scada Air.xlsx
+++ b/BoM Scada Air.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>No</t>
   </si>
@@ -135,6 +135,18 @@
   </si>
   <si>
     <t>NODE</t>
+  </si>
+  <si>
+    <t>modul charging</t>
+  </si>
+  <si>
+    <t>https://www.tokopedia.com/cncstorebandung/ups-module-18650-5v-3a-type-c-charge-discharging-highpower?extParam=whid%3D15512%26src%3Dchat</t>
+  </si>
+  <si>
+    <t>baterai</t>
+  </si>
+  <si>
+    <t>https://www.tokopedia.com/perfexstar/battery-baterai-sony-vtc5-18650-2600mah-30amax-original-authentic?extParam=ivf%3Dfalse&amp;src=topads</t>
   </si>
 </sst>
 </file>
@@ -202,12 +214,14 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -215,14 +229,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -504,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -519,16 +536,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -590,7 +607,7 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1">
-        <f t="shared" ref="F4:F16" si="0">C4*D4</f>
+        <f t="shared" ref="F4:F18" si="0">C4*D4</f>
         <v>6600</v>
       </c>
       <c r="G4" s="1"/>
@@ -848,6 +865,45 @@
       <c r="G16" s="1"/>
       <c r="H16" s="2" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="7">
+        <v>1</v>
+      </c>
+      <c r="D17" s="7">
+        <v>67000</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="7">
+        <f t="shared" si="0"/>
+        <v>67000</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="4">
+        <v>2</v>
+      </c>
+      <c r="D18" s="4">
+        <v>80000</v>
+      </c>
+      <c r="F18" s="4">
+        <f t="shared" si="0"/>
+        <v>160000</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -864,11 +920,13 @@
     <hyperlink ref="H9" r:id="rId7"/>
     <hyperlink ref="H10" r:id="rId8"/>
     <hyperlink ref="H11" r:id="rId9"/>
-    <hyperlink ref="H12"/>
+    <hyperlink ref="H12" display="https://www.tokopedia.com/arduinoid/pcf8575-remote-16-bits-i2c-smbus-i-o-expander-gpio-expansion-module?utm_campaign=PDP-28025336-11795598871-061223&amp;utm_source=salinlink&amp;utm_medium=share&amp;_branch_match_id=944048539765275900&amp;_branch_referrer=H4sIAAAAAAAAA8s"/>
     <hyperlink ref="H13" r:id="rId10"/>
     <hyperlink ref="H14" r:id="rId11"/>
     <hyperlink ref="H15" r:id="rId12"/>
     <hyperlink ref="H16" r:id="rId13"/>
+    <hyperlink ref="H17" r:id="rId14"/>
+    <hyperlink ref="H18" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>